<commit_message>
Fixed an equation issue in Line. Power flow matches MATPOWER.
</commit_message>
<xml_diff>
--- a/tests/pjm5bus.xlsx
+++ b/tests/pjm5bus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDA5566-1B0E-514B-B899-97205FDD5FB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1991E5-B7A1-5149-AED8-97100D29D844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="1480" windowWidth="32360" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="1480" windowWidth="32360" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -712,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
@@ -2097,9 +2097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2213,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -2266,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -2319,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -2372,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed initial value issue with bus voltages. Working Kundur systems
</commit_message>
<xml_diff>
--- a/tests/pjm5bus.xlsx
+++ b/tests/pjm5bus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1991E5-B7A1-5149-AED8-97100D29D844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82325B0-3C87-B64E-8B23-8B61510B6690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="1480" windowWidth="32360" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23080" windowHeight="13000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="82">
   <si>
     <t>idx</t>
   </si>
@@ -63,27 +63,15 @@
     <t>area</t>
   </si>
   <si>
+    <t>zone</t>
+  </si>
+  <si>
     <t>owner</t>
   </si>
   <si>
     <t>uid</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Bus 1</t>
   </si>
   <si>
@@ -201,12 +189,6 @@
     <t>phi</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Line 1-2</t>
   </si>
   <si>
@@ -231,33 +213,33 @@
     <t>gen</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>xl</t>
+  </si>
+  <si>
+    <t>xq</t>
+  </si>
+  <si>
+    <t>kp</t>
+  </si>
+  <si>
+    <t>kw</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
     <t>coi</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>xl</t>
-  </si>
-  <si>
-    <t>xq</t>
-  </si>
-  <si>
-    <t>kp</t>
-  </si>
-  <si>
-    <t>kw</t>
-  </si>
-  <si>
-    <t>S10</t>
-  </si>
-  <si>
-    <t>S12</t>
-  </si>
-  <si>
     <t>syn</t>
   </si>
   <si>
@@ -292,9 +274,6 @@
   </si>
   <si>
     <t>Line</t>
-  </si>
-  <si>
-    <t>zone</t>
   </si>
 </sst>
 </file>
@@ -326,7 +305,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -349,27 +328,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -714,14 +679,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -757,24 +722,24 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>230</v>
@@ -805,14 +770,14 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>230</v>
@@ -843,14 +808,14 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
+      <c r="B4">
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>230</v>
@@ -881,14 +846,14 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
+      <c r="B5">
+        <v>3</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>230</v>
@@ -919,14 +884,14 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
+      <c r="B6">
+        <v>4</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>230</v>
@@ -964,14 +929,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -983,16 +948,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -1000,25 +965,28 @@
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>3</v>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>230</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -1032,25 +1000,25 @@
       <c r="J2">
         <v>0.9</v>
       </c>
-      <c r="K2">
-        <v>230</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>230</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -1064,25 +1032,25 @@
       <c r="J3">
         <v>0.9</v>
       </c>
-      <c r="K3">
-        <v>230</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
+      <c r="B4">
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>230</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -1095,9 +1063,6 @@
       </c>
       <c r="J4">
         <v>0.9</v>
-      </c>
-      <c r="K4">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1111,14 +1076,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1130,34 +1095,34 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>6</v>
@@ -1169,24 +1134,24 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1194,8 +1159,8 @@
       <c r="F2">
         <v>230</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
+      <c r="G2">
+        <v>0</v>
       </c>
       <c r="I2">
         <v>2.1</v>
@@ -1235,14 +1200,14 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -1250,8 +1215,8 @@
       <c r="F3">
         <v>230</v>
       </c>
-      <c r="G3" t="s">
-        <v>15</v>
+      <c r="G3">
+        <v>2</v>
       </c>
       <c r="I3">
         <v>3.2349000000000001</v>
@@ -1291,14 +1256,14 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
+      <c r="B4">
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -1306,8 +1271,8 @@
       <c r="F4">
         <v>230</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4">
+        <v>4</v>
       </c>
       <c r="I4">
         <v>4.6650999999999998</v>
@@ -1354,14 +1319,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1373,34 +1338,34 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>6</v>
@@ -1412,10 +1377,10 @@
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>7</v>
@@ -1425,14 +1390,14 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
+      <c r="B2">
+        <v>3</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1440,8 +1405,8 @@
       <c r="F2">
         <v>230</v>
       </c>
-      <c r="G2" t="s">
-        <v>16</v>
+      <c r="G2">
+        <v>3</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1491,77 +1456,77 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I8"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>8</v>
@@ -1574,20 +1539,20 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
+        <v>53</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -1639,20 +1604,20 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
+        <v>54</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -1704,20 +1669,20 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
+      <c r="B4">
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
+        <v>55</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -1769,20 +1734,20 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
+      <c r="B5">
+        <v>3</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
+        <v>56</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -1834,20 +1799,20 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
+      <c r="B6">
+        <v>4</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
+        <v>57</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -1899,20 +1864,20 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>57</v>
+      <c r="B7">
+        <v>5</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
+        <v>58</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
       </c>
       <c r="G7">
         <v>100</v>
@@ -1964,20 +1929,20 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>58</v>
+      <c r="B8">
+        <v>6</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
+        <v>59</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
       </c>
       <c r="G8">
         <v>100</v>
@@ -2043,7 +2008,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2097,16 +2062,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S5" sqref="S5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2118,154 +2083,154 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="I2">
-        <v>230</v>
+        <v>60</v>
       </c>
       <c r="J2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="O2">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
       </c>
       <c r="H3">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="I3">
-        <v>230</v>
+        <v>60</v>
       </c>
       <c r="J3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="O3">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
         <v>1</v>
       </c>
     </row>
@@ -2273,52 +2238,52 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
+      <c r="B4">
+        <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="I4">
-        <v>230</v>
+        <v>60</v>
       </c>
       <c r="J4">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="O4">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
         <v>1</v>
       </c>
     </row>
@@ -2326,52 +2291,52 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
+      <c r="B5">
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
       </c>
       <c r="H5">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="I5">
-        <v>230</v>
+        <v>60</v>
       </c>
       <c r="J5">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="O5">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
         <v>1</v>
       </c>
     </row>
@@ -2382,18 +2347,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2405,57 +2370,54 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
+      <c r="E2">
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0.05</v>
       </c>
       <c r="G2">
-        <v>2.1040000000000001</v>
+        <v>999</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2478,22 +2440,19 @@
       <c r="N2">
         <v>10</v>
       </c>
-      <c r="O2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
+      <c r="B3">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
+      <c r="E3">
+        <v>2</v>
       </c>
       <c r="F3">
         <v>0.05</v>
@@ -2522,22 +2481,19 @@
       <c r="N3">
         <v>10</v>
       </c>
-      <c r="O3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
+      <c r="B4">
+        <v>3</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
+      <c r="E4">
+        <v>3</v>
       </c>
       <c r="F4">
         <v>0.05</v>
@@ -2566,22 +2522,19 @@
       <c r="N4">
         <v>10</v>
       </c>
-      <c r="O4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
+      <c r="B5">
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
+      <c r="E5">
+        <v>4</v>
       </c>
       <c r="F5">
         <v>0.05</v>
@@ -2609,9 +2562,6 @@
       </c>
       <c r="N5">
         <v>10</v>
-      </c>
-      <c r="O5">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2625,14 +2575,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2644,30 +2594,30 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
+        <v>81</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
       </c>
       <c r="G2">
         <v>2</v>

</xml_diff>